<commit_message>
Updating BOMs, starting new board.
</commit_message>
<xml_diff>
--- a/adapter_board/EasyLink_AdatperBoard_v1/EasyLink_AdapterBoard_v1_BOM.xlsx
+++ b/adapter_board/EasyLink_AdatperBoard_v1/EasyLink_AdapterBoard_v1_BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F561B3D4-CCBC-4E96-8D9B-AFB1FC292CA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23923B02-8D87-417E-94C0-701FC8780EA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Designator</t>
   </si>
@@ -58,7 +58,13 @@
     <t>CONN HDR 10POS 0.1 GOLD PCB R/A</t>
   </si>
   <si>
-    <t>Reset button</t>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>TL3365AF180QG</t>
+  </si>
+  <si>
+    <t>EG5384CT-ND</t>
   </si>
 </sst>
 </file>
@@ -379,7 +385,7 @@
   <dimension ref="A3:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B6" sqref="B6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +450,12 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>